<commit_message>
individual and complete benchmarks completed
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios_24_06.xlsx
+++ b/test/inputs/Scenarios_24_06.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47802FD2-F02D-46D5-80CF-AFE4651EC950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725E7D0C-1B37-495A-A464-23A0489A9384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="18240" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="549">
   <si>
     <t>input_file</t>
   </si>
@@ -1675,6 +1675,12 @@
   </si>
   <si>
     <t>Benchmark_All_Metabo</t>
+  </si>
+  <si>
+    <t>Benchmark_All_Water</t>
+  </si>
+  <si>
+    <t>Benchmark_All_Growth</t>
   </si>
 </sst>
 </file>
@@ -2858,11 +2864,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O219"/>
+  <dimension ref="A1:Q219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J7" sqref="J7"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2872,10 +2878,10 @@
     <col min="5" max="5" width="58.109375" customWidth="1"/>
     <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.5546875" style="37" customWidth="1"/>
-    <col min="8" max="15" width="39.88671875" style="1" customWidth="1"/>
+    <col min="8" max="17" width="39.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>469</v>
       </c>
@@ -2907,22 +2913,28 @@
         <v>546</v>
       </c>
       <c r="K1" s="36" t="s">
+        <v>547</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>548</v>
+      </c>
+      <c r="M1" s="36" t="s">
         <v>512</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="N1" s="36" t="s">
         <v>524</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="O1" s="36" t="s">
         <v>525</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>538</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="Q1" s="36" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>541</v>
       </c>
@@ -2954,10 +2966,10 @@
         <v>545</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>476</v>
+        <v>545</v>
       </c>
       <c r="L2" s="36" t="s">
-        <v>476</v>
+        <v>545</v>
       </c>
       <c r="M2" s="36" t="s">
         <v>476</v>
@@ -2968,8 +2980,14 @@
       <c r="O2" s="36" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P2" s="36" t="s">
+        <v>476</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>472</v>
       </c>
@@ -3001,10 +3019,10 @@
         <v>489</v>
       </c>
       <c r="K3" s="36" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="L3" s="36" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="M3" s="36" t="s">
         <v>489</v>
@@ -3015,8 +3033,14 @@
       <c r="O3" s="36" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="36" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>484</v>
       </c>
@@ -3048,10 +3072,10 @@
         <v>482</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="L4" s="36" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="M4" s="36" t="s">
         <v>482</v>
@@ -3062,8 +3086,14 @@
       <c r="O4" s="36" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="36" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q4" s="36" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>483</v>
       </c>
@@ -3095,10 +3125,10 @@
         <v>494</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="L5" s="36" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="M5" s="36" t="s">
         <v>494</v>
@@ -3109,8 +3139,14 @@
       <c r="O5" s="36" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="36" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q5" s="36" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>490</v>
       </c>
@@ -3142,10 +3178,10 @@
         <v>476</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>537</v>
+        <v>476</v>
       </c>
       <c r="L6" s="36" t="s">
-        <v>537</v>
+        <v>476</v>
       </c>
       <c r="M6" s="36" t="s">
         <v>537</v>
@@ -3156,8 +3192,14 @@
       <c r="O6" s="36" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P6" s="36" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q6" s="36" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>485</v>
       </c>
@@ -3192,7 +3234,7 @@
         <v>494</v>
       </c>
       <c r="L7" s="36" t="s">
-        <v>494</v>
+        <v>476</v>
       </c>
       <c r="M7" s="36" t="s">
         <v>494</v>
@@ -3203,8 +3245,14 @@
       <c r="O7" s="36" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="36" t="s">
+        <v>494</v>
+      </c>
+      <c r="Q7" s="36" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -3250,8 +3298,14 @@
       <c r="O8" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q8" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -3297,8 +3351,14 @@
       <c r="O9" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="74" t="s">
         <v>444</v>
       </c>
@@ -3344,8 +3404,14 @@
       <c r="O10" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -3391,8 +3457,14 @@
       <c r="O11" s="85">
         <v>180</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="85">
+        <v>180</v>
+      </c>
+      <c r="Q11" s="85">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -3438,8 +3510,14 @@
       <c r="O12" s="78">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="78">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="Q12" s="78">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -3485,8 +3563,14 @@
       <c r="O13" s="79">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="79">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="Q13" s="79">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
@@ -3532,8 +3616,14 @@
       <c r="O14" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>448</v>
       </c>
@@ -3579,8 +3669,14 @@
       <c r="O15" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P15" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
@@ -3626,8 +3722,14 @@
       <c r="O16" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q16" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>7</v>
       </c>
@@ -3673,8 +3775,14 @@
       <c r="O17" s="80">
         <v>5.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="80">
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="Q17" s="80">
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -3720,8 +3828,14 @@
       <c r="O18" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="77">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>461</v>
       </c>
@@ -3767,8 +3881,14 @@
       <c r="O19" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q19" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>462</v>
       </c>
@@ -3814,8 +3934,14 @@
       <c r="O20" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q20" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>465</v>
       </c>
@@ -3861,8 +3987,14 @@
       <c r="O21" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q21" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>467</v>
       </c>
@@ -3908,8 +4040,14 @@
       <c r="O22" s="77">
         <v>86400</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="77">
+        <v>86400</v>
+      </c>
+      <c r="Q22" s="77">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
@@ -3940,11 +4078,11 @@
       <c r="J23" s="85" t="b">
         <v>0</v>
       </c>
-      <c r="K23" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="L23" s="77" t="s">
-        <v>87</v>
+      <c r="K23" s="85" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" s="85" t="b">
+        <v>0</v>
       </c>
       <c r="M23" s="77" t="s">
         <v>87</v>
@@ -3955,8 +4093,14 @@
       <c r="O23" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q23" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
@@ -4002,8 +4146,14 @@
       <c r="O24" s="77">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="77">
+        <v>3</v>
+      </c>
+      <c r="Q24" s="77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>363</v>
       </c>
@@ -4049,8 +4199,14 @@
       <c r="O25" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q25" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>365</v>
       </c>
@@ -4096,8 +4252,14 @@
       <c r="O26" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q26" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>377</v>
       </c>
@@ -4143,8 +4305,14 @@
       <c r="O27" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q27" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>376</v>
       </c>
@@ -4190,8 +4358,14 @@
       <c r="O28" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q28" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>375</v>
       </c>
@@ -4237,8 +4411,14 @@
       <c r="O29" s="81" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q29" s="81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>12</v>
       </c>
@@ -4284,8 +4464,14 @@
       <c r="O30" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q30" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>13</v>
       </c>
@@ -4331,8 +4517,14 @@
       <c r="O31" s="77">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P31" s="77">
+        <v>0.33</v>
+      </c>
+      <c r="Q31" s="77">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>14</v>
       </c>
@@ -4378,8 +4570,14 @@
       <c r="O32" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q32" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>9</v>
       </c>
@@ -4425,8 +4623,14 @@
       <c r="O33" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P33" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q33" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>454</v>
       </c>
@@ -4472,8 +4676,14 @@
       <c r="O34" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P34" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q34" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>21</v>
       </c>
@@ -4519,8 +4729,14 @@
       <c r="O35" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P35" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q35" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>22</v>
       </c>
@@ -4566,8 +4782,14 @@
       <c r="O36" s="85" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P36" s="85" t="s">
+        <v>433</v>
+      </c>
+      <c r="Q36" s="85" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>23</v>
       </c>
@@ -4613,8 +4835,14 @@
       <c r="O37" s="80">
         <v>9.9999999999999995E-7</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="80">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="Q37" s="80">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>24</v>
       </c>
@@ -4660,8 +4888,14 @@
       <c r="O38" s="86">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P38" s="86">
+        <v>1E-3</v>
+      </c>
+      <c r="Q38" s="86">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>25</v>
       </c>
@@ -4707,8 +4941,14 @@
       <c r="O39" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P39" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q39" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>26</v>
       </c>
@@ -4754,8 +4994,14 @@
       <c r="O40" s="77" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P40" s="77" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q40" s="77" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>27</v>
       </c>
@@ -4801,8 +5047,14 @@
       <c r="O41" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P41" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q41" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>28</v>
       </c>
@@ -4848,8 +5100,14 @@
       <c r="O42" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q42" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>29</v>
       </c>
@@ -4895,8 +5153,14 @@
       <c r="O43" s="77">
         <v>120</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P43" s="77">
+        <v>120</v>
+      </c>
+      <c r="Q43" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>30</v>
       </c>
@@ -4942,8 +5206,14 @@
       <c r="O44" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P44" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>31</v>
       </c>
@@ -4989,8 +5259,14 @@
       <c r="O45" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P45" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>32</v>
       </c>
@@ -5036,8 +5312,14 @@
       <c r="O46" s="77">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P46" s="77">
+        <v>-0.1</v>
+      </c>
+      <c r="Q46" s="77">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>33</v>
       </c>
@@ -5083,8 +5365,14 @@
       <c r="O47" s="77">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P47" s="77">
+        <v>-0.2</v>
+      </c>
+      <c r="Q47" s="77">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>34</v>
       </c>
@@ -5130,8 +5418,14 @@
       <c r="O48" s="77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P48" s="77">
+        <v>0.4</v>
+      </c>
+      <c r="Q48" s="77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>35</v>
       </c>
@@ -5177,8 +5471,14 @@
       <c r="O49" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P49" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>434</v>
       </c>
@@ -5224,8 +5524,14 @@
       <c r="O50" s="77">
         <v>1200</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P50" s="77">
+        <v>1200</v>
+      </c>
+      <c r="Q50" s="77">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>435</v>
       </c>
@@ -5271,8 +5577,14 @@
       <c r="O51" s="77">
         <v>1200</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P51" s="77">
+        <v>1200</v>
+      </c>
+      <c r="Q51" s="77">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>457</v>
       </c>
@@ -5318,8 +5630,14 @@
       <c r="O52" s="35" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P52" s="35" t="s">
+        <v>460</v>
+      </c>
+      <c r="Q52" s="35" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>15</v>
       </c>
@@ -5365,8 +5683,14 @@
       <c r="O53" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P53" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q53" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>16</v>
       </c>
@@ -5412,8 +5736,14 @@
       <c r="O54" s="77" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P54" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q54" s="77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>17</v>
       </c>
@@ -5459,8 +5789,14 @@
       <c r="O55" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P55" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>18</v>
       </c>
@@ -5506,8 +5842,14 @@
       <c r="O56" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P56" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="Q56" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>19</v>
       </c>
@@ -5553,8 +5895,14 @@
       <c r="O57" s="77">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P57" s="77">
+        <v>0.05</v>
+      </c>
+      <c r="Q57" s="77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>36</v>
       </c>
@@ -5600,8 +5948,14 @@
       <c r="O58" s="80">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P58" s="80">
+        <v>1E-3</v>
+      </c>
+      <c r="Q58" s="80">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>380</v>
       </c>
@@ -5647,8 +6001,14 @@
       <c r="O59" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P59" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>37</v>
       </c>
@@ -5694,8 +6054,14 @@
       <c r="O60" s="77">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P60" s="77">
+        <v>1E-4</v>
+      </c>
+      <c r="Q60" s="77">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>38</v>
       </c>
@@ -5741,8 +6107,14 @@
       <c r="O61" s="77">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P61" s="77">
+        <v>1E-4</v>
+      </c>
+      <c r="Q61" s="77">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>39</v>
       </c>
@@ -5788,8 +6160,14 @@
       <c r="O62" s="77">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P62" s="77">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="Q62" s="77">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>40</v>
       </c>
@@ -5835,8 +6213,14 @@
       <c r="O63" s="77">
         <v>1.22E-4</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P63" s="77">
+        <v>1.22E-4</v>
+      </c>
+      <c r="Q63" s="77">
+        <v>1.22E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>207</v>
       </c>
@@ -5882,8 +6266,14 @@
       <c r="O64" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P64" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q64" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>41</v>
       </c>
@@ -5929,8 +6319,14 @@
       <c r="O65" s="77">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P65" s="77">
+        <v>0.95</v>
+      </c>
+      <c r="Q65" s="77">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>406</v>
       </c>
@@ -5976,8 +6372,14 @@
       <c r="O66" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P66" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q66" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
         <v>91</v>
       </c>
@@ -6023,8 +6425,14 @@
       <c r="O67" s="77">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P67" s="77">
+        <v>5</v>
+      </c>
+      <c r="Q67" s="77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>408</v>
       </c>
@@ -6070,8 +6478,14 @@
       <c r="O68" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P68" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q68" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>42</v>
       </c>
@@ -6117,8 +6531,14 @@
       <c r="O69" s="77">
         <v>50</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P69" s="77">
+        <v>50</v>
+      </c>
+      <c r="Q69" s="77">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
         <v>208</v>
       </c>
@@ -6164,8 +6584,14 @@
       <c r="O70" s="78">
         <v>1453890.8941884842</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P70" s="78">
+        <v>1453890.8941884842</v>
+      </c>
+      <c r="Q70" s="78">
+        <v>1453890.8941884842</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
         <v>43</v>
       </c>
@@ -6211,8 +6637,14 @@
       <c r="O71" s="78">
         <v>1.3888888888888888E-5</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P71" s="78">
+        <v>1.3888888888888888E-5</v>
+      </c>
+      <c r="Q71" s="78">
+        <v>1.3888888888888888E-5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>44</v>
       </c>
@@ -6258,8 +6690,14 @@
       <c r="O72" s="79">
         <v>6.5011574074074071E-4</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P72" s="79">
+        <v>6.5011574074074071E-4</v>
+      </c>
+      <c r="Q72" s="79">
+        <v>6.5011574074074071E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
         <v>45</v>
       </c>
@@ -6305,8 +6743,14 @@
       <c r="O73" s="85">
         <v>4.7400000000000003E-3</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P73" s="85">
+        <v>4.7400000000000003E-3</v>
+      </c>
+      <c r="Q73" s="85">
+        <v>4.7400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="17" t="s">
         <v>46</v>
       </c>
@@ -6352,8 +6796,14 @@
       <c r="O74" s="79">
         <v>282528</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P74" s="79">
+        <v>282528</v>
+      </c>
+      <c r="Q74" s="79">
+        <v>282528</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
         <v>47</v>
       </c>
@@ -6399,8 +6849,14 @@
       <c r="O75" s="85">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P75" s="85">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="Q75" s="85">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
         <v>48</v>
       </c>
@@ -6446,8 +6902,14 @@
       <c r="O76" s="87">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P76" s="87">
+        <v>0.16</v>
+      </c>
+      <c r="Q76" s="87">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
         <v>49</v>
       </c>
@@ -6493,8 +6955,14 @@
       <c r="O77" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P77" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>50</v>
       </c>
@@ -6540,8 +7008,14 @@
       <c r="O78" s="78">
         <v>745476480000</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P78" s="78">
+        <v>745476480000</v>
+      </c>
+      <c r="Q78" s="78">
+        <v>745476480000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
         <v>205</v>
       </c>
@@ -6587,8 +7061,14 @@
       <c r="O79" s="77">
         <v>100</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P79" s="77">
+        <v>100</v>
+      </c>
+      <c r="Q79" s="77">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
         <v>414</v>
       </c>
@@ -6620,10 +7100,10 @@
         <v>87</v>
       </c>
       <c r="K80" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L80" s="77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M80" s="77" t="s">
         <v>88</v>
@@ -6634,8 +7114,14 @@
       <c r="O80" s="77" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P80" s="77" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q80" s="77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
         <v>400</v>
       </c>
@@ -6681,8 +7167,14 @@
       <c r="O81" s="85">
         <v>21600</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P81" s="85">
+        <v>21600</v>
+      </c>
+      <c r="Q81" s="85">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
         <v>410</v>
       </c>
@@ -6728,8 +7220,14 @@
       <c r="O82" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P82" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="Q82" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
         <v>401</v>
       </c>
@@ -6775,8 +7273,14 @@
       <c r="O83" s="85">
         <v>60479.999999999993</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P83" s="85">
+        <v>60479.999999999993</v>
+      </c>
+      <c r="Q83" s="85">
+        <v>60479.999999999993</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="33" t="s">
         <v>411</v>
       </c>
@@ -6822,8 +7326,14 @@
       <c r="O84" s="77">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P84" s="77">
+        <v>0.85</v>
+      </c>
+      <c r="Q84" s="77">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="33" t="s">
         <v>402</v>
       </c>
@@ -6869,8 +7379,14 @@
       <c r="O85" s="77">
         <v>518400</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P85" s="77">
+        <v>518400</v>
+      </c>
+      <c r="Q85" s="77">
+        <v>518400</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="33" t="s">
         <v>412</v>
       </c>
@@ -6916,8 +7432,14 @@
       <c r="O86" s="77">
         <v>5184000</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P86" s="77">
+        <v>5184000</v>
+      </c>
+      <c r="Q86" s="77">
+        <v>5184000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
         <v>51</v>
       </c>
@@ -6963,8 +7485,14 @@
       <c r="O87" s="86">
         <v>50000</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P87" s="86">
+        <v>50000</v>
+      </c>
+      <c r="Q87" s="86">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>52</v>
       </c>
@@ -7010,8 +7538,14 @@
       <c r="O88" s="77">
         <v>140000</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P88" s="77">
+        <v>140000</v>
+      </c>
+      <c r="Q88" s="77">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
         <v>53</v>
       </c>
@@ -7057,8 +7591,14 @@
       <c r="O89" s="78">
         <v>3.6636136999999999E-2</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P89" s="78">
+        <v>3.6636136999999999E-2</v>
+      </c>
+      <c r="Q89" s="78">
+        <v>3.6636136999999999E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
         <v>54</v>
       </c>
@@ -7104,8 +7644,14 @@
       <c r="O90" s="77">
         <v>4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P90" s="77">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="Q90" s="77">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="17" t="s">
         <v>55</v>
       </c>
@@ -7137,10 +7683,10 @@
         <v>0.06</v>
       </c>
       <c r="K91" s="77">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="L91" s="77">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="M91" s="77">
         <v>0.05</v>
@@ -7151,8 +7697,14 @@
       <c r="O91" s="77">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P91" s="77">
+        <v>0.05</v>
+      </c>
+      <c r="Q91" s="77">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>214</v>
       </c>
@@ -7198,8 +7750,14 @@
       <c r="O92" s="77">
         <v>6.0000000000000002E-6</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P92" s="77">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="Q92" s="77">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>215</v>
       </c>
@@ -7240,13 +7798,19 @@
         <v>1E-3</v>
       </c>
       <c r="N93" s="77">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="O93" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1E-3</v>
+      </c>
+      <c r="P93" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>216</v>
       </c>
@@ -7292,8 +7856,14 @@
       <c r="O94" s="77">
         <v>374999999.99999994</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P94" s="77">
+        <v>374999999.99999994</v>
+      </c>
+      <c r="Q94" s="77">
+        <v>374999999.99999994</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>217</v>
       </c>
@@ -7339,8 +7909,14 @@
       <c r="O95" s="78">
         <v>3.7037037037037038E-3</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P95" s="78">
+        <v>3.7037037037037038E-3</v>
+      </c>
+      <c r="Q95" s="78">
+        <v>3.7037037037037038E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="19" t="s">
         <v>218</v>
       </c>
@@ -7386,8 +7962,14 @@
       <c r="O96" s="77">
         <v>165600</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P96" s="77">
+        <v>165600</v>
+      </c>
+      <c r="Q96" s="77">
+        <v>165600</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>60</v>
       </c>
@@ -7433,8 +8015,14 @@
       <c r="O97" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P97" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q97" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>209</v>
       </c>
@@ -7480,8 +8068,14 @@
       <c r="O98" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P98" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q98" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>59</v>
       </c>
@@ -7527,8 +8121,14 @@
       <c r="O99" s="77">
         <v>21</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P99" s="77">
+        <v>21</v>
+      </c>
+      <c r="Q99" s="77">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" s="23" t="s">
         <v>65</v>
       </c>
@@ -7574,8 +8174,14 @@
       <c r="O100" s="77">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P100" s="77">
+        <v>0.64</v>
+      </c>
+      <c r="Q100" s="77">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" s="23" t="s">
         <v>367</v>
       </c>
@@ -7621,8 +8227,14 @@
       <c r="O101" s="77">
         <v>8</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P101" s="77">
+        <v>8</v>
+      </c>
+      <c r="Q101" s="77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>368</v>
       </c>
@@ -7668,8 +8280,14 @@
       <c r="O102" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P102" s="77">
+        <v>10</v>
+      </c>
+      <c r="Q102" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
         <v>369</v>
       </c>
@@ -7715,8 +8333,14 @@
       <c r="O103" s="77">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P103" s="77">
+        <v>8</v>
+      </c>
+      <c r="Q103" s="77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
         <v>505</v>
       </c>
@@ -7762,8 +8386,14 @@
       <c r="O104" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P104" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q104" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" s="23" t="s">
         <v>385</v>
       </c>
@@ -7809,8 +8439,14 @@
       <c r="O105" s="77">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P105" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="Q105" s="77">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" s="23" t="s">
         <v>506</v>
       </c>
@@ -7830,7 +8466,7 @@
         <v>511</v>
       </c>
       <c r="G106" s="58">
-        <f t="shared" ref="G106:M106" si="0">G104</f>
+        <f t="shared" ref="G106:O106" si="0">G104</f>
         <v>1</v>
       </c>
       <c r="H106" s="58">
@@ -7842,15 +8478,15 @@
         <v>1</v>
       </c>
       <c r="J106" s="58">
-        <f t="shared" ref="J106" si="1">J104</f>
+        <f t="shared" ref="J106:K106" si="1">J104</f>
         <v>1</v>
       </c>
       <c r="K106" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L106" s="58">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L106" si="2">L104</f>
         <v>1</v>
       </c>
       <c r="M106" s="58">
@@ -7858,13 +8494,21 @@
         <v>1</v>
       </c>
       <c r="N106" s="58">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O106" s="58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P106" s="58">
+        <v>1</v>
+      </c>
+      <c r="Q106" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" s="23" t="s">
         <v>507</v>
       </c>
@@ -7888,37 +8532,45 @@
         <v>3</v>
       </c>
       <c r="H107" s="58">
-        <f t="shared" ref="H107:M107" si="2">150*H104</f>
+        <f t="shared" ref="H107:O107" si="3">150*H104</f>
         <v>150</v>
       </c>
       <c r="I107" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="J107" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="K107" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K107:L107" si="4">150*K104</f>
         <v>150</v>
       </c>
       <c r="L107" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="M107" s="58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="N107" s="58">
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="O107" s="58">
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P107" s="58">
+        <v>150</v>
+      </c>
+      <c r="Q107" s="58">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" s="23" t="s">
         <v>508</v>
       </c>
@@ -7938,41 +8590,49 @@
         <v>511</v>
       </c>
       <c r="G108" s="58">
-        <f t="shared" ref="G108:M108" si="3">G99</f>
+        <f t="shared" ref="G108:O108" si="5">G99</f>
         <v>21</v>
       </c>
       <c r="H108" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="I108" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J108" s="58">
-        <f t="shared" ref="J108" si="4">J99</f>
+        <f t="shared" ref="J108:K108" si="6">J99</f>
         <v>21</v>
       </c>
       <c r="K108" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="L108" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L108" si="7">L99</f>
         <v>21</v>
       </c>
       <c r="M108" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="N108" s="58">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="O108" s="58">
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P108" s="58">
+        <v>21</v>
+      </c>
+      <c r="Q108" s="58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" s="23" t="s">
         <v>509</v>
       </c>
@@ -7996,37 +8656,45 @@
         <v>210</v>
       </c>
       <c r="H109" s="58">
-        <f t="shared" ref="H109:M109" si="5">70*H99</f>
+        <f t="shared" ref="H109:O109" si="8">70*H99</f>
         <v>1470</v>
       </c>
       <c r="I109" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1470</v>
       </c>
       <c r="J109" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1470</v>
       </c>
       <c r="K109" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K109:L109" si="9">70*K99</f>
         <v>1470</v>
       </c>
       <c r="L109" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1470</v>
       </c>
       <c r="M109" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1470</v>
       </c>
       <c r="N109" s="58">
+        <f t="shared" si="8"/>
         <v>1470</v>
       </c>
       <c r="O109" s="58">
+        <f t="shared" si="8"/>
         <v>1470</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P109" s="58">
+        <v>1470</v>
+      </c>
+      <c r="Q109" s="58">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" s="23" t="s">
         <v>387</v>
       </c>
@@ -8072,8 +8740,14 @@
       <c r="O110" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P110" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q110" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" s="23" t="s">
         <v>389</v>
       </c>
@@ -8119,8 +8793,14 @@
       <c r="O111" s="82">
         <v>1589759.9999999998</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P111" s="82">
+        <v>1589759.9999999998</v>
+      </c>
+      <c r="Q111" s="82">
+        <v>1589759.9999999998</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" s="23" t="s">
         <v>391</v>
       </c>
@@ -8166,8 +8846,14 @@
       <c r="O112" s="82">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P112" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+      <c r="Q112" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" s="23" t="s">
         <v>393</v>
       </c>
@@ -8213,8 +8899,14 @@
       <c r="O113" s="82">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P113" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+      <c r="Q113" s="82">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" s="23" t="s">
         <v>421</v>
       </c>
@@ -8260,8 +8952,14 @@
       <c r="O114" s="82">
         <v>100</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P114" s="82">
+        <v>100</v>
+      </c>
+      <c r="Q114" s="82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="23" t="s">
         <v>423</v>
       </c>
@@ -8285,37 +8983,45 @@
         <v>280800</v>
       </c>
       <c r="H115" s="67">
-        <f t="shared" ref="H115:M115" si="6">0.1 * 3.25 * (60*60*24)</f>
+        <f t="shared" ref="H115:O115" si="10">0.1 * 3.25 * (60*60*24)</f>
         <v>28080</v>
       </c>
       <c r="I115" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
       <c r="J115" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
       <c r="K115" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
       <c r="L115" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
       <c r="M115" s="67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
       <c r="N115" s="67">
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
       <c r="O115" s="67">
+        <f t="shared" si="10"/>
         <v>28080</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P115" s="67">
+        <v>28080</v>
+      </c>
+      <c r="Q115" s="67">
+        <v>28080</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" s="23" t="s">
         <v>425</v>
       </c>
@@ -8339,37 +9045,45 @@
         <v>1.2847222222222224E-5</v>
       </c>
       <c r="H116" s="67">
-        <f t="shared" ref="H116:M116" si="7">1.11 / 10</f>
+        <f t="shared" ref="H116:O116" si="11">1.11 / 10</f>
         <v>0.11100000000000002</v>
       </c>
       <c r="I116" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="J116" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="K116" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="L116" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="M116" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="N116" s="67">
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
       <c r="O116" s="67">
+        <f t="shared" si="11"/>
         <v>0.11100000000000002</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P116" s="67">
+        <v>0.11100000000000002</v>
+      </c>
+      <c r="Q116" s="67">
+        <v>0.11100000000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" s="23" t="s">
         <v>502</v>
       </c>
@@ -8415,8 +9129,14 @@
       <c r="O117" s="82">
         <v>100</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="P117" s="82">
+        <v>100</v>
+      </c>
+      <c r="Q117" s="82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="23" t="s">
         <v>503</v>
       </c>
@@ -8436,41 +9156,49 @@
         <v>431</v>
       </c>
       <c r="G118" s="67">
-        <f t="shared" ref="G118:M118" si="8">5.32 * (60*60*24)</f>
+        <f t="shared" ref="G118:O118" si="12">5.32 * (60*60*24)</f>
         <v>459648</v>
       </c>
       <c r="H118" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="I118" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="J118" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="K118" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="L118" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="M118" s="67">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="N118" s="67">
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
       <c r="O118" s="67">
+        <f t="shared" si="12"/>
         <v>459648</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P118" s="67">
+        <v>459648</v>
+      </c>
+      <c r="Q118" s="67">
+        <v>459648</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" s="23" t="s">
         <v>504</v>
       </c>
@@ -8494,37 +9222,45 @@
         <v>1.2847222222222224E-5</v>
       </c>
       <c r="H119" s="67">
-        <f t="shared" ref="H119:M119" si="9">1.11/8</f>
+        <f t="shared" ref="H119:O119" si="13">1.11/8</f>
         <v>0.13875000000000001</v>
       </c>
       <c r="I119" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="J119" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="K119" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="L119" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="M119" s="67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="N119" s="67">
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
       <c r="O119" s="67">
+        <f t="shared" si="13"/>
         <v>0.13875000000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P119" s="67">
+        <v>0.13875000000000001</v>
+      </c>
+      <c r="Q119" s="67">
+        <v>0.13875000000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" s="23" t="s">
         <v>395</v>
       </c>
@@ -8570,8 +9306,14 @@
       <c r="O120" s="82">
         <v>21600</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P120" s="82">
+        <v>21600</v>
+      </c>
+      <c r="Q120" s="82">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" s="23" t="s">
         <v>397</v>
       </c>
@@ -8617,8 +9359,14 @@
       <c r="O121" s="88">
         <v>43200</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P121" s="88">
+        <v>43200</v>
+      </c>
+      <c r="Q121" s="88">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" s="13" t="s">
         <v>61</v>
       </c>
@@ -8664,8 +9412,14 @@
       <c r="O122" s="77">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P122" s="77">
+        <v>0.8</v>
+      </c>
+      <c r="Q122" s="77">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
         <v>62</v>
       </c>
@@ -8700,9 +9454,11 @@
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="K123" s="78">
+        <f>1250*0.000001/6</f>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="L123" s="78">
+        <f>1250*0.000001/6</f>
         <v>2.0833333333333335E-4</v>
       </c>
       <c r="M123" s="78">
@@ -8714,8 +9470,14 @@
       <c r="O123" s="78">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P123" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+      <c r="Q123" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
         <v>63</v>
       </c>
@@ -8761,8 +9523,14 @@
       <c r="O124" s="77">
         <v>5.7899999999999998E-7</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P124" s="77">
+        <v>5.7899999999999998E-7</v>
+      </c>
+      <c r="Q124" s="77">
+        <v>5.7899999999999998E-7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
         <v>64</v>
       </c>
@@ -8808,8 +9576,14 @@
       <c r="O125" s="78">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P125" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+      <c r="Q125" s="78">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
         <v>450</v>
       </c>
@@ -8855,8 +9629,14 @@
       <c r="O126" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P126" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" s="13" t="s">
         <v>452</v>
       </c>
@@ -8902,8 +9682,14 @@
       <c r="O127" s="78">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P127" s="78">
+        <v>0</v>
+      </c>
+      <c r="Q127" s="78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" s="68" t="s">
         <v>441</v>
       </c>
@@ -8947,8 +9733,14 @@
       <c r="O128" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P128" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" s="68" t="s">
         <v>67</v>
       </c>
@@ -8992,8 +9784,14 @@
       <c r="O129" s="89">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P129" s="89">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" s="68" t="s">
         <v>446</v>
       </c>
@@ -9039,8 +9837,14 @@
       <c r="O130" s="89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P130" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q130" s="89" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
         <v>66</v>
       </c>
@@ -9086,8 +9890,14 @@
       <c r="O131" s="83">
         <v>5.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P131" s="83">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="Q131" s="83">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
         <v>438</v>
       </c>
@@ -9133,8 +9943,14 @@
       <c r="O132" s="83">
         <v>4.9999999999999999E-13</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P132" s="83">
+        <v>4.9999999999999999E-13</v>
+      </c>
+      <c r="Q132" s="83">
+        <v>4.9999999999999999E-13</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
         <v>229</v>
       </c>
@@ -9180,8 +9996,14 @@
       <c r="O133" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P133" s="77">
+        <v>10</v>
+      </c>
+      <c r="Q133" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
         <v>230</v>
       </c>
@@ -9227,8 +10049,14 @@
       <c r="O134" s="77">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P134" s="77">
+        <v>-0.04</v>
+      </c>
+      <c r="Q134" s="77">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" s="21" t="s">
         <v>231</v>
       </c>
@@ -9274,8 +10102,14 @@
       <c r="O135" s="77">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P135" s="77">
+        <v>2.9</v>
+      </c>
+      <c r="Q135" s="77">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" s="21" t="s">
         <v>232</v>
       </c>
@@ -9321,8 +10155,14 @@
       <c r="O136" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P136" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q136" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" s="21" t="s">
         <v>68</v>
       </c>
@@ -9368,8 +10208,14 @@
       <c r="O137" s="80">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P137" s="80">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="Q137" s="80">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="s">
         <v>233</v>
       </c>
@@ -9415,8 +10261,14 @@
       <c r="O138" s="77">
         <v>10</v>
       </c>
-    </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P138" s="77">
+        <v>10</v>
+      </c>
+      <c r="Q138" s="77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" s="21" t="s">
         <v>234</v>
       </c>
@@ -9462,8 +10314,14 @@
       <c r="O139" s="77">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P139" s="77">
+        <v>-0.04</v>
+      </c>
+      <c r="Q139" s="77">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
         <v>235</v>
       </c>
@@ -9509,8 +10367,14 @@
       <c r="O140" s="77">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P140" s="77">
+        <v>2.9</v>
+      </c>
+      <c r="Q140" s="77">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
         <v>236</v>
       </c>
@@ -9556,8 +10420,14 @@
       <c r="O141" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P141" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q141" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" s="21" t="s">
         <v>69</v>
       </c>
@@ -9603,8 +10473,14 @@
       <c r="O142" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P142" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q142" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" s="72" t="s">
         <v>70</v>
       </c>
@@ -9650,8 +10526,14 @@
       <c r="O143" s="80">
         <v>5.0000000000000004E-6</v>
       </c>
-    </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P143" s="80">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="Q143" s="80">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" s="23" t="s">
         <v>56</v>
       </c>
@@ -9697,8 +10579,14 @@
       <c r="O144" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P144" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q144" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" s="23" t="s">
         <v>57</v>
       </c>
@@ -9744,8 +10632,14 @@
       <c r="O145" s="77">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P145" s="77">
+        <v>2E-3</v>
+      </c>
+      <c r="Q145" s="77">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" s="23" t="s">
         <v>58</v>
       </c>
@@ -9791,8 +10685,14 @@
       <c r="O146" s="80">
         <v>3.9999999999999998E-6</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P146" s="80">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="Q146" s="80">
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" s="23" t="s">
         <v>71</v>
       </c>
@@ -9838,8 +10738,14 @@
       <c r="O147" s="80">
         <v>3.7699999999999999E-10</v>
       </c>
-    </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P147" s="80">
+        <v>3.7699999999999999E-10</v>
+      </c>
+      <c r="Q147" s="80">
+        <v>3.7699999999999999E-10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" s="23" t="s">
         <v>237</v>
       </c>
@@ -9885,8 +10791,14 @@
       <c r="O148" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P148" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q148" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" s="23" t="s">
         <v>238</v>
       </c>
@@ -9932,8 +10844,14 @@
       <c r="O149" s="77">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P149" s="77">
+        <v>-0.06</v>
+      </c>
+      <c r="Q149" s="77">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" s="23" t="s">
         <v>239</v>
       </c>
@@ -9979,8 +10897,14 @@
       <c r="O150" s="77">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P150" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="Q150" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" s="23" t="s">
         <v>240</v>
       </c>
@@ -10026,8 +10950,14 @@
       <c r="O151" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P151" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q151" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" s="23" t="s">
         <v>72</v>
       </c>
@@ -10073,8 +11003,14 @@
       <c r="O152" s="80">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P152" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="Q152" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" s="13" t="s">
         <v>73</v>
       </c>
@@ -10120,8 +11056,14 @@
       <c r="O153" s="80">
         <v>5.8333333333333335E-9</v>
       </c>
-    </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P153" s="80">
+        <v>5.8333333333333335E-9</v>
+      </c>
+      <c r="Q153" s="80">
+        <v>5.8333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" s="13" t="s">
         <v>241</v>
       </c>
@@ -10167,8 +11109,14 @@
       <c r="O154" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P154" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q154" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" s="13" t="s">
         <v>242</v>
       </c>
@@ -10214,8 +11162,14 @@
       <c r="O155" s="77">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P155" s="77">
+        <v>-0.06</v>
+      </c>
+      <c r="Q155" s="77">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
         <v>243</v>
       </c>
@@ -10261,8 +11215,14 @@
       <c r="O156" s="77">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P156" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="Q156" s="77">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
         <v>244</v>
       </c>
@@ -10308,8 +11268,14 @@
       <c r="O157" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P157" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q157" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" s="13" t="s">
         <v>74</v>
       </c>
@@ -10355,8 +11321,14 @@
       <c r="O158" s="80">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P158" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="Q158" s="80">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="s">
         <v>75</v>
       </c>
@@ -10402,8 +11374,14 @@
       <c r="O159" s="83">
         <v>4.0000000000000001E-8</v>
       </c>
-    </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P159" s="83">
+        <v>4.0000000000000001E-8</v>
+      </c>
+      <c r="Q159" s="83">
+        <v>4.0000000000000001E-8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>219</v>
       </c>
@@ -10449,8 +11427,14 @@
       <c r="O160" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P160" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q160" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
         <v>220</v>
       </c>
@@ -10496,8 +11480,14 @@
       <c r="O161" s="77">
         <v>-4.4200000000000003E-2</v>
       </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P161" s="77">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+      <c r="Q161" s="77">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
         <v>221</v>
       </c>
@@ -10543,8 +11533,14 @@
       <c r="O162" s="77">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P162" s="77">
+        <v>1.55</v>
+      </c>
+      <c r="Q162" s="77">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>222</v>
       </c>
@@ -10590,8 +11586,14 @@
       <c r="O163" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P163" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q163" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" s="9" t="s">
         <v>76</v>
       </c>
@@ -10637,8 +11639,14 @@
       <c r="O164" s="77">
         <v>2.7799999999999998E-4</v>
       </c>
-    </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P164" s="77">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="Q164" s="77">
+        <v>2.7799999999999998E-4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" s="25" t="s">
         <v>78</v>
       </c>
@@ -10670,11 +11678,9 @@
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="K165" s="84">
-        <f>H165</f>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="L165" s="84">
-        <f>H165</f>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="M165" s="84">
@@ -10682,13 +11688,21 @@
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="N165" s="84">
+        <f>H165</f>
         <v>2.4999999999999998E-12</v>
       </c>
       <c r="O165" s="84">
+        <f>H165</f>
         <v>2.4999999999999998E-12</v>
       </c>
-    </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P165" s="84">
+        <v>2.4999999999999998E-12</v>
+      </c>
+      <c r="Q165" s="84">
+        <v>2.4999999999999998E-12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" s="25" t="s">
         <v>246</v>
       </c>
@@ -10734,8 +11748,14 @@
       <c r="O166" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P166" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q166" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" s="25" t="s">
         <v>247</v>
       </c>
@@ -10781,8 +11801,14 @@
       <c r="O167" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P167" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q167" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A168" s="25" t="s">
         <v>248</v>
       </c>
@@ -10828,8 +11854,14 @@
       <c r="O168" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P168" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q168" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" s="25" t="s">
         <v>249</v>
       </c>
@@ -10875,8 +11907,14 @@
       <c r="O169" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P169" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q169" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" s="25" t="s">
         <v>79</v>
       </c>
@@ -10922,8 +11960,14 @@
       <c r="O170" s="77">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P170" s="77">
+        <v>0.4</v>
+      </c>
+      <c r="Q170" s="77">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" s="31" t="s">
         <v>80</v>
       </c>
@@ -10969,8 +12013,14 @@
       <c r="O171" s="86">
         <v>2.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P171" s="86">
+        <v>2.0000000000000001E-9</v>
+      </c>
+      <c r="Q171" s="86">
+        <v>2.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" s="31" t="s">
         <v>250</v>
       </c>
@@ -11016,8 +12066,14 @@
       <c r="O172" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P172" s="77">
+        <v>25</v>
+      </c>
+      <c r="Q172" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>251</v>
       </c>
@@ -11063,8 +12119,14 @@
       <c r="O173" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P173" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q173" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" s="31" t="s">
         <v>252</v>
       </c>
@@ -11110,8 +12172,14 @@
       <c r="O174" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P174" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="Q174" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" s="31" t="s">
         <v>253</v>
       </c>
@@ -11157,8 +12225,14 @@
       <c r="O175" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P175" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q175" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" s="31" t="s">
         <v>81</v>
       </c>
@@ -11204,8 +12278,14 @@
       <c r="O176" s="78">
         <v>1.6666666666666666E-4</v>
       </c>
-    </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P176" s="78">
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="Q176" s="78">
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" s="11" t="s">
         <v>254</v>
       </c>
@@ -11251,8 +12331,14 @@
       <c r="O177" s="80">
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P177" s="80">
+        <v>1E-8</v>
+      </c>
+      <c r="Q177" s="80">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" s="11" t="s">
         <v>255</v>
       </c>
@@ -11298,8 +12384,14 @@
       <c r="O178" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P178" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q178" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
         <v>256</v>
       </c>
@@ -11345,8 +12437,14 @@
       <c r="O179" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P179" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q179" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" s="11" t="s">
         <v>257</v>
       </c>
@@ -11392,8 +12490,14 @@
       <c r="O180" s="77">
         <v>2</v>
       </c>
-    </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P180" s="77">
+        <v>2</v>
+      </c>
+      <c r="Q180" s="77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
         <v>258</v>
       </c>
@@ -11439,8 +12543,14 @@
       <c r="O181" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P181" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q181" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
         <v>259</v>
       </c>
@@ -11486,8 +12596,14 @@
       <c r="O182" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P182" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="Q182" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" s="11" t="s">
         <v>260</v>
       </c>
@@ -11533,8 +12649,14 @@
       <c r="O183" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P183" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q183" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" s="27" t="s">
         <v>261</v>
       </c>
@@ -11580,8 +12702,14 @@
       <c r="O184" s="77">
         <v>2.3533050791148899E-8</v>
       </c>
-    </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P184" s="77">
+        <v>2.3533050791148899E-8</v>
+      </c>
+      <c r="Q184" s="77">
+        <v>2.3533050791148899E-8</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" s="27" t="s">
         <v>262</v>
       </c>
@@ -11627,8 +12755,14 @@
       <c r="O185" s="77">
         <v>20</v>
       </c>
-    </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P185" s="77">
+        <v>20</v>
+      </c>
+      <c r="Q185" s="77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" s="27" t="s">
         <v>263</v>
       </c>
@@ -11674,8 +12808,14 @@
       <c r="O186" s="77">
         <v>-0.187</v>
       </c>
-    </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P186" s="77">
+        <v>-0.187</v>
+      </c>
+      <c r="Q186" s="77">
+        <v>-0.187</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" s="27" t="s">
         <v>264</v>
       </c>
@@ -11721,8 +12861,14 @@
       <c r="O187" s="77">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P187" s="77">
+        <v>2.48</v>
+      </c>
+      <c r="Q187" s="77">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" s="27" t="s">
         <v>265</v>
       </c>
@@ -11768,8 +12914,14 @@
       <c r="O188" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P188" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q188" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" s="27" t="s">
         <v>266</v>
       </c>
@@ -11815,8 +12967,14 @@
       <c r="O189" s="77">
         <v>6.1060227588121015E-4</v>
       </c>
-    </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P189" s="77">
+        <v>6.1060227588121015E-4</v>
+      </c>
+      <c r="Q189" s="77">
+        <v>6.1060227588121015E-4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" s="23" t="s">
         <v>267</v>
       </c>
@@ -11862,8 +13020,14 @@
       <c r="O190" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P190" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="Q190" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" s="23" t="s">
         <v>268</v>
       </c>
@@ -11909,8 +13073,14 @@
       <c r="O191" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P191" s="77">
+        <v>25</v>
+      </c>
+      <c r="Q191" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" s="23" t="s">
         <v>269</v>
       </c>
@@ -11956,8 +13126,14 @@
       <c r="O192" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P192" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q192" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" s="23" t="s">
         <v>270</v>
       </c>
@@ -12003,8 +13179,14 @@
       <c r="O193" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P193" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="Q193" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" s="23" t="s">
         <v>271</v>
       </c>
@@ -12050,8 +13232,14 @@
       <c r="O194" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P194" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q194" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" s="23" t="s">
         <v>272</v>
       </c>
@@ -12097,8 +13285,14 @@
       <c r="O195" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P195" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="Q195" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>273</v>
       </c>
@@ -12144,8 +13338,14 @@
       <c r="O196" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P196" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="Q196" s="85">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>274</v>
       </c>
@@ -12191,8 +13391,14 @@
       <c r="O197" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P197" s="77">
+        <v>25</v>
+      </c>
+      <c r="Q197" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>275</v>
       </c>
@@ -12238,8 +13444,14 @@
       <c r="O198" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P198" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q198" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>276</v>
       </c>
@@ -12285,8 +13497,14 @@
       <c r="O199" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P199" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="Q199" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>277</v>
       </c>
@@ -12332,8 +13550,14 @@
       <c r="O200" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P200" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q200" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
         <v>278</v>
       </c>
@@ -12379,8 +13603,14 @@
       <c r="O201" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P201" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="Q201" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" s="29" t="s">
         <v>279</v>
       </c>
@@ -12426,8 +13656,14 @@
       <c r="O202" s="85">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P202" s="85">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="Q202" s="85">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" s="29" t="s">
         <v>280</v>
       </c>
@@ -12473,8 +13709,14 @@
       <c r="O203" s="77">
         <v>25</v>
       </c>
-    </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P203" s="77">
+        <v>25</v>
+      </c>
+      <c r="Q203" s="77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" s="29" t="s">
         <v>281</v>
       </c>
@@ -12520,8 +13762,14 @@
       <c r="O204" s="77">
         <v>0</v>
       </c>
-    </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P204" s="77">
+        <v>0</v>
+      </c>
+      <c r="Q204" s="77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" s="29" t="s">
         <v>282</v>
       </c>
@@ -12567,8 +13815,14 @@
       <c r="O205" s="77">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P205" s="77">
+        <v>3.98</v>
+      </c>
+      <c r="Q205" s="77">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
         <v>283</v>
       </c>
@@ -12614,8 +13868,14 @@
       <c r="O206" s="77">
         <v>1</v>
       </c>
-    </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P206" s="77">
+        <v>1</v>
+      </c>
+      <c r="Q206" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" s="29" t="s">
         <v>284</v>
       </c>
@@ -12661,8 +13921,14 @@
       <c r="O207" s="78">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P207" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="Q207" s="78">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" s="90" t="s">
         <v>362</v>
       </c>
@@ -12708,8 +13974,14 @@
       <c r="O208" s="95" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="209" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P208" s="95" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q208" s="95" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="209" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>495</v>
       </c>
@@ -12741,22 +14013,28 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="K209" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L209" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M209" s="2">
         <v>0.01</v>
-      </c>
-      <c r="L209" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="M209" s="2">
-        <v>1</v>
       </c>
       <c r="N209" s="2">
         <v>0.01</v>
       </c>
       <c r="O209" s="2">
+        <v>1</v>
+      </c>
+      <c r="P209" s="2">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="210" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q209" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="210" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>499</v>
       </c>
@@ -12788,10 +14066,10 @@
         <v>-100000</v>
       </c>
       <c r="K210" s="98">
-        <v>0</v>
+        <v>-100000</v>
       </c>
       <c r="L210" s="98">
-        <v>0</v>
+        <v>-100000</v>
       </c>
       <c r="M210" s="98">
         <v>0</v>
@@ -12802,8 +14080,14 @@
       <c r="O210" s="98">
         <v>0</v>
       </c>
-    </row>
-    <row r="211" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P210" s="98">
+        <v>0</v>
+      </c>
+      <c r="Q210" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>522</v>
       </c>
@@ -12826,37 +14110,45 @@
         <v>-100000</v>
       </c>
       <c r="H211" s="98">
-        <f t="shared" ref="H211:M211" si="10">H210</f>
+        <f t="shared" ref="H211:O211" si="14">H210</f>
         <v>-100000</v>
       </c>
       <c r="I211" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-100000</v>
       </c>
       <c r="J211" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-100000</v>
       </c>
       <c r="K211" s="98">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" ref="K211:L211" si="15">K210</f>
+        <v>-100000</v>
       </c>
       <c r="L211" s="98">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="15"/>
+        <v>-100000</v>
       </c>
       <c r="M211" s="98">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="N211" s="98">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="O211" s="98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="P211" s="98">
+        <v>0</v>
+      </c>
+      <c r="Q211" s="98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>513</v>
       </c>
@@ -12888,22 +14180,28 @@
         <v>0.5</v>
       </c>
       <c r="K212" s="99">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L212" s="99">
+        <v>0.5</v>
+      </c>
+      <c r="M212" s="99">
+        <v>1</v>
+      </c>
+      <c r="N212" s="99">
         <v>0.01</v>
       </c>
-      <c r="M212" s="99">
-        <v>1</v>
-      </c>
-      <c r="N212" s="99">
-        <v>1</v>
-      </c>
       <c r="O212" s="99">
+        <v>1</v>
+      </c>
+      <c r="P212" s="99">
+        <v>1</v>
+      </c>
+      <c r="Q212" s="99">
         <v>0.01</v>
       </c>
     </row>
-    <row r="213" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>514</v>
       </c>
@@ -12934,23 +14232,29 @@
       <c r="J213" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="K213" s="97">
+      <c r="K213" s="99" t="s">
+        <v>476</v>
+      </c>
+      <c r="L213" s="99" t="s">
+        <v>476</v>
+      </c>
+      <c r="M213" s="97">
         <v>0.1</v>
       </c>
-      <c r="L213" s="97" t="s">
-        <v>476</v>
-      </c>
-      <c r="M213" s="97" t="s">
-        <v>476</v>
-      </c>
-      <c r="N213" s="97">
+      <c r="N213" s="97" t="s">
+        <v>476</v>
+      </c>
+      <c r="O213" s="97" t="s">
+        <v>476</v>
+      </c>
+      <c r="P213" s="97">
         <v>0.1</v>
       </c>
-      <c r="O213" s="97" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="214" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q213" s="97" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>515</v>
       </c>
@@ -12981,11 +14285,11 @@
       <c r="J214" s="99">
         <v>0</v>
       </c>
-      <c r="K214" s="97">
-        <v>0.04</v>
-      </c>
-      <c r="L214" s="97">
-        <v>0.04</v>
+      <c r="K214" s="99">
+        <v>0</v>
+      </c>
+      <c r="L214" s="99">
+        <v>0</v>
       </c>
       <c r="M214" s="97">
         <v>0.04</v>
@@ -12996,8 +14300,14 @@
       <c r="O214" s="97">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="215" spans="1:15" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P214" s="97">
+        <v>0.04</v>
+      </c>
+      <c r="Q214" s="97">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" s="96" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>516</v>
       </c>
@@ -13028,10 +14338,10 @@
       <c r="J215" s="99">
         <v>1E-3</v>
       </c>
-      <c r="K215" s="97">
+      <c r="K215" s="99">
         <v>1E-3</v>
       </c>
-      <c r="L215" s="97">
+      <c r="L215" s="99">
         <v>1E-3</v>
       </c>
       <c r="M215" s="97">
@@ -13043,8 +14353,14 @@
       <c r="O215" s="97">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P215" s="97">
+        <v>1E-3</v>
+      </c>
+      <c r="Q215" s="97">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>526</v>
       </c>
@@ -13090,8 +14406,14 @@
       <c r="O216" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P216" s="2">
+        <v>29</v>
+      </c>
+      <c r="Q216" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>528</v>
       </c>
@@ -13127,25 +14449,33 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K217" s="98">
+        <f>1250*0.000001/5</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="L217" s="98">
+        <f>1250*0.000001/5</f>
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="M217" s="98">
         <f>H217</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="L217" s="98">
-        <f t="shared" ref="L217:M217" si="11">K217</f>
+      <c r="N217" s="98">
+        <f t="shared" ref="N217:O217" si="16">M217</f>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="M217" s="98">
-        <f t="shared" si="11"/>
+      <c r="O217" s="98">
+        <f t="shared" si="16"/>
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="N217" s="98">
+      <c r="P217" s="98">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="O217" s="98">
+      <c r="Q217" s="98">
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>531</v>
       </c>
@@ -13191,8 +14521,14 @@
       <c r="O218" s="99">
         <v>9.9999999999999994E-12</v>
       </c>
-    </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P218" s="99">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="Q218" s="99">
+        <v>9.9999999999999994E-12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>534</v>
       </c>
@@ -13238,9 +14574,15 @@
       <c r="O219" s="98">
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="P219" s="98">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="Q219" s="98">
+        <v>2.0000000000000001E-4</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H126:M127">
+  <conditionalFormatting sqref="H126:O127">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -13252,7 +14594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H131:O131">
+  <conditionalFormatting sqref="H131:Q131">
     <cfRule type="colorScale" priority="229">
       <colorScale>
         <cfvo type="min"/>
@@ -13274,7 +14616,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H132:O132">
+  <conditionalFormatting sqref="H132:Q132">
     <cfRule type="colorScale" priority="231">
       <colorScale>
         <cfvo type="min"/>
@@ -13296,7 +14638,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H137:O137">
+  <conditionalFormatting sqref="H137:Q137">
     <cfRule type="colorScale" priority="233">
       <colorScale>
         <cfvo type="min"/>
@@ -13308,7 +14650,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H143:O143">
+  <conditionalFormatting sqref="H143:Q143">
     <cfRule type="colorScale" priority="234">
       <colorScale>
         <cfvo type="min"/>
@@ -13340,7 +14682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H159:O159">
+  <conditionalFormatting sqref="H159:Q159">
     <cfRule type="colorScale" priority="237">
       <colorScale>
         <cfvo type="min"/>
@@ -13372,7 +14714,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H165:O165">
+  <conditionalFormatting sqref="H165:Q165">
     <cfRule type="colorScale" priority="240">
       <colorScale>
         <cfvo type="min"/>
@@ -13404,7 +14746,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N126:O127">
+  <conditionalFormatting sqref="P126:Q127">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>